<commit_message>
More work with templates
</commit_message>
<xml_diff>
--- a/Template.xlsx
+++ b/Template.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="FMEA" sheetId="1" r:id="rId1"/>
+    <sheet name="COMPONENTS" sheetId="2" r:id="rId1"/>
+    <sheet name="FMEA" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -474,6 +475,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">

</xml_diff>